<commit_message>
bleu score implemented again, normalized var (?) during eval, added prefix and graph to dictionary, created eval runner file which needs to be implemented to allow fast experimentation
</commit_message>
<xml_diff>
--- a/experiments/results/terms_vs_embs.xlsx
+++ b/experiments/results/terms_vs_embs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\32472\Desktop\MaastrichtUni\Year3\ThesisSep\CodeDataFinal\nl2sparql-thesis\experiments\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C4869D0-F961-4323-AD24-835222425C8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE3CB32A-1444-45E0-8ADC-29C5551D3B50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1820" yWindow="1820" windowWidth="19200" windowHeight="11170" xr2:uid="{FC4796CB-7247-4160-AFC0-215DCB58961B}"/>
+    <workbookView xWindow="6420" yWindow="380" windowWidth="12980" windowHeight="15370" xr2:uid="{FC4796CB-7247-4160-AFC0-215DCB58961B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -50,13 +50,19 @@
     <t>with_embeddings</t>
   </si>
   <si>
-    <t>PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
-PREFIX cdio: &lt;https://w3id.org/CDIO/&gt;
-PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
-PREFIX ns1: &lt;http://purl.obolibrary.org/obo/bfo.owl#&gt;
-PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
-PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt;
-SELECT DISTINCT ?study 
+    <t>with_onehop</t>
+  </si>
+  <si>
+    <t>with_onehop_terms_embs</t>
+  </si>
+  <si>
+    <t>with_nhop</t>
+  </si>
+  <si>
+    <t>with_nhop_terms_embs</t>
+  </si>
+  <si>
+    <t>SELECT DISTINCT ?study 
 WHERE {
   GRAPH &lt;https://w3id.org/CDIO/graph/studies&gt; {
     ?study a obi:study_design_execution ;
@@ -78,13 +84,7 @@
 }</t>
   </si>
   <si>
-    <t>prefix bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
-prefix cdio: &lt;https://w3id.org/CDIO/&gt;
-prefix dc: &lt;http://purl.org/dc/elements/1.1/&gt;
-prefix ns1: &lt;http://purl.obolibrary.org/obo/bfo.owl#&gt;
-prefix obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
-prefix xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt;
-SELECT DISTINCT ?study 
+    <t>SELECT DISTINCT ?study 
 WHERE {
   GRAPH &lt;https://w3id.org/CDIO/graph/studies&gt; {
     ?study a obi:study_design_execution ;
@@ -106,13 +106,7 @@
 }</t>
   </si>
   <si>
-    <t>prefix bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
-prefix cdio: &lt;https://w3id.org/CDIO/&gt;
-prefix dc: &lt;http://purl.org/dc/elements/1.1/&gt;
-prefix ns1: &lt;http://purl.obolibrary.org/obo/bfo.owl#&gt;
-prefix obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
-prefix xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt;
-SELECT (COUNT(?data_element) AS ?var_count)
+    <t>SELECT (COUNT(?data_element) AS ?var_count)
 WHERE {
     GRAPH &lt;https://w3id.org/CDIO/graph/studies&gt;{
          ?study a obi:study_design_execution ;
@@ -126,13 +120,7 @@
 }</t>
   </si>
   <si>
-    <t>prefix bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
-prefix cdio: &lt;https://w3id.org/CDIO/&gt;
-prefix dc: &lt;http://purl.org/dc/elements/1.1/&gt;
-prefix ns1: &lt;http://purl.obolibrary.org/obo/bfo.owl#&gt;
-prefix obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
-prefix xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt;
-SELECT (COUNT(?data_element) AS ?var_count)
+    <t>SELECT (COUNT(?data_element) AS ?var_count)
 WHERE {
     GRAPH &lt;https://w3id.org/CDIO/graph/studies&gt;{
          ?study a obi:study_design_execution ;
@@ -153,11 +141,7 @@
 }</t>
   </si>
   <si>
-    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
-PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt;
-PREFIX dct: &lt;http://purl.org/dc/terms/&gt;
-PREFIX cdio: &lt;https://w3id.org/CDIO/time-chf/&gt;
-SELECT DISTINCT ?study ?title ?description
+    <t>SELECT DISTINCT ?study ?title ?description
 WHERE {
   ?study rdf:type ?type ;
          dct:title ?title ;
@@ -176,21 +160,63 @@
 }</t>
   </si>
   <si>
-    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
-PREFIX cdio: &lt;https://w3id.org/CDIO/&gt;
-SELECT DISTINCT ?study
+    <t>SELECT DISTINCT ?study
 WHERE {
   ?study rdf:type cdio:Study .
   ?study cdio:hasDisease &lt;https://w3id.org/CDIO/time-chf/diabetes&gt; .
 }</t>
   </si>
   <si>
-    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
-PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt;
-PREFIX sio: &lt;http://semanticscience.org/resource/&gt;
-PREFIX obo: &lt;http://purl.obolibrary.org/obo/&gt;
-PREFIX cdio: &lt;https://w3id.org/CDIO/&gt;
-SELECT DISTINCT ?study ?studyLabel
+    <t>SELECT DISTINCT ?study
+WHERE {
+  VALUES ?disease { cdio:diabetes }
+  ?disease cdio:study_design_variable_specification ?spec1 .
+  ?spec1 ?p1 cdio:%25406mwt .
+  cdio:%25406mwt cdio:study_design_variable_specification ?spec2 .
+  ?spec2 ?p2 cdio:gdsbl .
+  cdio:gdsbl cdio:study_design_variable_specification ?study .
+}</t>
+  </si>
+  <si>
+    <t>SELECT DISTINCT ?study ?studyTitle ?disease
+WHERE {
+  ?study rdf:type schema:MedicalStudy .
+  ?study schema:about ?disease .
+  FILTER(
+    ?disease IN (
+      cdio:diabetes,
+      cdio:diabetesaes,
+      cdio:firstdiabetesae,
+      cdio:maxdiabetesaeseverity,
+      cdio:sumdiabetesaeseverity,
+      cdio:totaldurationdiabetes
+    )
+  )
+  OPTIONAL { ?study dct:title ?studyTitle . }
+}
+ORDER BY ?studyTitle</t>
+  </si>
+  <si>
+    <t>SELECT DISTINCT ?study
+WHERE {
+  ?study a cdio:study_design_execution .
+  ?study bfo:concretizes ?design .
+  ?design bfo:has_part ?protocol .
+  ?protocol bfo:has_part ?variableSpec .
+  ?variableSpec bfo:has_part cdio:diabetes .
+}</t>
+  </si>
+  <si>
+    <t>SELECT DISTINCT ?study
+WHERE {
+  ?study bfo:has_part ?study_design .
+  ?study_design bfo:has_part ?protocol .
+  ?protocol bfo:has_part ?variable_spec .
+  ?variable_spec bfo:has_part &lt;https://w3id.org/CDIO/time-chf/diabetes&gt; .
+}</t>
+  </si>
+  <si>
+    <t>SELECT DISTINCT ?study ?studyLabel
 WHERE {
   ?study rdf:type sio:Study .
   ?study rdfs:label ?studyLabel .
@@ -205,10 +231,7 @@
 ORDER BY ?studyLabel</t>
   </si>
   <si>
-    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
-PREFIX cdio: &lt;https://w3id.org/CDIO/cardiateam/&gt;
-PREFIX timechf: &lt;https://w3id.org/CDIO/time-chf/&gt;
-SELECT DISTINCT ?study ?label
+    <t>SELECT DISTINCT ?study ?label
 WHERE {
   ?study rdf:type cdio:study_design_execution .
   ?study rdfs:label ?label .
@@ -230,118 +253,7 @@
 }</t>
   </si>
   <si>
-    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
-SELECT (COUNT(DISTINCT ?variable) AS ?variableCount)
-WHERE {
-  VALUES ?study {
-    &lt;https://w3id.org/CDIO/time-chf/study_design_variable_specification&gt;
-  }
-  ?variable rdf:type ?study .
-}</t>
-  </si>
-  <si>
-    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
-SELECT (COUNT(?variable) AS ?count)
-WHERE {
-  VALUES ?study { &lt;https://w3id.org/CDIO/time-chf/hr&gt; &lt;https://w3id.org/CDIO/time-chf/a&gt; &lt;https://w3id.org/CDIO/time-chf/hct&gt; &lt;https://w3id.org/CDIO/time-chf/ec&gt; &lt;https://w3id.org/CDIO/time-chf/hrecg&gt; &lt;https://w3id.org/CDIO/time-chf/ti&gt; &lt;https://w3id.org/CDIO/time-chf/e&gt; &lt;https://w3id.org/CDIO/time-chf/hct6&gt; &lt;https://w3id.org/CDIO/time-chf/hr6&gt; &lt;https://w3id.org/CDIO/time-chf/protocol&gt; &lt;https://w3id.org/CDIO/time-chf/v12&gt; &lt;https://w3id.org/CDIO/time-chf/hr1&gt; &lt;https://w3id.org/CDIO/time-chf/lc&gt; &lt;https://w3id.org/CDIO/time-chf/py&gt; &lt;https://w3id.org/CDIO/time-chf/ms&gt; &lt;https://w3id.org/CDIO/time-chf/ec6&gt; &lt;https://w3id.org/CDIO/time-chf/v6&gt; &lt;https://w3id.org/CDIO/time-chf/hr3&gt; &lt;https://w3id.org/CDIO/time-chf/v3&gt; &lt;https://w3id.org/CDIO/time-chf/hr12&gt; &lt;https://w3id.org/CDIO/time-chf/pc6&gt; &lt;https://w3id.org/CDIO/time-chf/alt&gt; }
-  ?variable rdf:subject ?study .
-}</t>
-  </si>
-  <si>
-    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
-PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt;
-PREFIX cdio: &lt;https://w3id.org/CDIO/time-chf/&gt;
-SELECT (COUNT(?var) AS ?drugVariableCount)
-WHERE {
-  ?var rdf:type ?type .
-  ?var rdfs:label ?label .
-  FILTER(CONTAINS(LCASE(STR(?label)), "drug"))
-  FILTER(STRSTARTS(STR(?var), STR(cdio:)))
-}</t>
-  </si>
-  <si>
-    <t>PREFIX cdio: &lt;https://w3id.org/CDIO/&gt;
-PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt;
-SELECT (COUNT(?variable) AS ?drugVariableCount)
-WHERE {
-  ?variable rdfs:isDefinedBy &lt;https://w3id.org/CDIO/time-chf/&gt; .
-  ?variable cdio:has_value ?value .
-  FILTER(REGEX(STR(?variable), "drug", "i"))
-}</t>
-  </si>
-  <si>
-    <t>PREFIX cdio: &lt;https://w3id.org/CDIO/time-chf/&gt;
-SELECT DISTINCT ?study
-WHERE {
-  VALUES ?disease { cdio:diabetes }
-  ?disease cdio:study_design_variable_specification ?spec1 .
-  ?spec1 ?p1 cdio:%25406mwt .
-  cdio:%25406mwt cdio:study_design_variable_specification ?spec2 .
-  ?spec2 ?p2 cdio:gdsbl .
-  cdio:gdsbl cdio:study_design_variable_specification ?study .
-}</t>
-  </si>
-  <si>
-    <t>with_onehop</t>
-  </si>
-  <si>
-    <t>with_onehop_terms_embs</t>
-  </si>
-  <si>
-    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
-PREFIX cdio: &lt;https://w3id.org/CDIO/time-chf/&gt;
-PREFIX dct: &lt;http://purl.org/dc/terms/&gt;
-PREFIX schema: &lt;http://schema.org/&gt;
-SELECT DISTINCT ?study ?studyTitle ?disease
-WHERE {
-  ?study rdf:type schema:MedicalStudy .
-  ?study schema:about ?disease .
-  FILTER(
-    ?disease IN (
-      cdio:diabetes,
-      cdio:diabetesaes,
-      cdio:firstdiabetesae,
-      cdio:maxdiabetesaeseverity,
-      cdio:sumdiabetesaeseverity,
-      cdio:totaldurationdiabetes
-    )
-  )
-  OPTIONAL { ?study dct:title ?studyTitle . }
-}
-ORDER BY ?studyTitle</t>
-  </si>
-  <si>
-    <t>with_nhop</t>
-  </si>
-  <si>
-    <t>PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl#&gt;
-PREFIX cdio: &lt;https://w3id.org/CDIO/time-chf/&gt;
-SELECT DISTINCT ?study
-WHERE {
-  ?study a cdio:study_design_execution .
-  ?study bfo:concretizes ?design .
-  ?design bfo:has_part ?protocol .
-  ?protocol bfo:has_part ?variableSpec .
-  ?variableSpec bfo:has_part cdio:diabetes .
-}</t>
-  </si>
-  <si>
-    <t>with_nhop_terms_embs</t>
-  </si>
-  <si>
-    <t>PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl#&gt;
-PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
-SELECT DISTINCT ?study
-WHERE {
-  ?study bfo:has_part ?study_design .
-  ?study_design bfo:has_part ?protocol .
-  ?protocol bfo:has_part ?variable_spec .
-  ?variable_spec bfo:has_part &lt;https://w3id.org/CDIO/time-chf/diabetes&gt; .
-}</t>
-  </si>
-  <si>
-    <t>PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl#&gt;
-SELECT DISTINCT ?study
+    <t>SELECT DISTINCT ?study
 WHERE {
   ?study bfo:concretizes ?study_design_execution .
   ?study_design_execution bfo:concretizes &lt;https://w3id.org/CDIO/time-chf/study_design&gt; .
@@ -351,8 +263,23 @@
 }</t>
   </si>
   <si>
-    <t>PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl#&gt;
-SELECT (COUNT(DISTINCT ?variable) AS ?variableCount)
+    <t>SELECT (COUNT(DISTINCT ?variable) AS ?variableCount)
+WHERE {
+  VALUES ?study {
+    &lt;https://w3id.org/CDIO/time-chf/study_design_variable_specification&gt;
+  }
+  ?variable rdf:type ?study .
+}</t>
+  </si>
+  <si>
+    <t>SELECT (COUNT(?variable) AS ?count)
+WHERE {
+  VALUES ?study { &lt;https://w3id.org/CDIO/time-chf/hr&gt; &lt;https://w3id.org/CDIO/time-chf/a&gt; &lt;https://w3id.org/CDIO/time-chf/hct&gt; &lt;https://w3id.org/CDIO/time-chf/ec&gt; &lt;https://w3id.org/CDIO/time-chf/hrecg&gt; &lt;https://w3id.org/CDIO/time-chf/ti&gt; &lt;https://w3id.org/CDIO/time-chf/e&gt; &lt;https://w3id.org/CDIO/time-chf/hct6&gt; &lt;https://w3id.org/CDIO/time-chf/hr6&gt; &lt;https://w3id.org/CDIO/time-chf/protocol&gt; &lt;https://w3id.org/CDIO/time-chf/v12&gt; &lt;https://w3id.org/CDIO/time-chf/hr1&gt; &lt;https://w3id.org/CDIO/time-chf/lc&gt; &lt;https://w3id.org/CDIO/time-chf/py&gt; &lt;https://w3id.org/CDIO/time-chf/ms&gt; &lt;https://w3id.org/CDIO/time-chf/ec6&gt; &lt;https://w3id.org/CDIO/time-chf/v6&gt; &lt;https://w3id.org/CDIO/time-chf/hr3&gt; &lt;https://w3id.org/CDIO/time-chf/v3&gt; &lt;https://w3id.org/CDIO/time-chf/hr12&gt; &lt;https://w3id.org/CDIO/time-chf/pc6&gt; &lt;https://w3id.org/CDIO/time-chf/alt&gt; }
+  ?variable rdf:subject ?study .
+}</t>
+  </si>
+  <si>
+    <t>SELECT (COUNT(DISTINCT ?variable) AS ?variableCount)
 WHERE {
   &lt;https://w3id.org/CDIO/time-chf/study_design_execution&gt; 
       bfo:concretizes &lt;https://w3id.org/CDIO/time-chf/study_design&gt; .
@@ -365,10 +292,24 @@
 }</t>
   </si>
   <si>
-    <t>PREFIX cdio: &lt;https://w3id.org/CDIO/dysfunction-dm/&gt;
-PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
-PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt;
-SELECT (COUNT(DISTINCT ?variable) AS ?drugVariableCount)
+    <t>SELECT (COUNT(?var) AS ?drugVariableCount)
+WHERE {
+  ?var rdf:type ?type .
+  ?var rdfs:label ?label .
+  FILTER(CONTAINS(LCASE(STR(?label)), "drug"))
+  FILTER(STRSTARTS(STR(?var), STR(cdio:)))
+}</t>
+  </si>
+  <si>
+    <t>SELECT (COUNT(?variable) AS ?drugVariableCount)
+WHERE {
+  ?variable rdfs:isDefinedBy &lt;https://w3id.org/CDIO/time-chf/&gt; .
+  ?variable cdio:has_value ?value .
+  FILTER(REGEX(STR(?variable), "drug", "i"))
+}</t>
+  </si>
+  <si>
+    <t>SELECT (COUNT(DISTINCT ?variable) AS ?drugVariableCount)
 WHERE {
   ?study rdfs:label "time-chf" .
   ?study bfo:concretizes ?study_design_execution .
@@ -754,8 +695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{528626DB-76D5-4FF5-AF9C-7E3E0E09574C}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -783,16 +724,16 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
@@ -800,25 +741,25 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="H2" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
@@ -826,16 +767,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
@@ -843,16 +784,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
@@ -860,13 +801,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>26</v>

</xml_diff>